<commit_message>
update source for community developer
</commit_message>
<xml_diff>
--- a/RPATemplete/Data/Config.xlsx
+++ b/RPATemplete/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thaibev\RPATemplete\RPATemplete\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA869FC-EFD7-41F4-B486-4F4105BDF36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A8F9B4-8085-4138-91D3-FFDD7726D199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1164" windowWidth="17928" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -124,9 +124,6 @@
     <t>D:\RPA\{0}\process\{1}</t>
   </si>
   <si>
-    <t>path for process files</t>
-  </si>
-  <si>
     <t>sapUserName</t>
   </si>
   <si>
@@ -181,21 +178,12 @@
     <t>MailBody</t>
   </si>
   <si>
-    <t>[RPA_XXXXX] Master Templete on {0}</t>
-  </si>
-  <si>
     <t>MailFolderInbox</t>
   </si>
   <si>
-    <t>bots_SOP_inbox</t>
-  </si>
-  <si>
     <t>MailFolderMoveTo</t>
   </si>
   <si>
-    <t>bots_SOP</t>
-  </si>
-  <si>
     <t>ThaibevOACEmailPassword</t>
   </si>
   <si>
@@ -203,13 +191,33 @@
   </si>
   <si>
     <t xml:space="preserve">Dear All &lt;br/&gt;This is auto email from Master Templete Bot.&lt;br/&gt;Detail is : </t>
+  </si>
+  <si>
+    <t>inbox</t>
+  </si>
+  <si>
+    <t>bots</t>
+  </si>
+  <si>
+    <t>path for process files is details
+1. {0} get data from config excel value name is "ProcessName"
+2. {1} bot genarate from date now</t>
+  </si>
+  <si>
+    <t>[RPA_ProcessName] Master Templete on {0}</t>
+  </si>
+  <si>
+    <t>MailException</t>
+  </si>
+  <si>
+    <t>rpa@thaibev.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -233,6 +241,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -251,10 +265,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -264,8 +279,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -578,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -628,18 +645,18 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>30</v>
@@ -659,7 +676,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.4">
+    <row r="5" spans="1:26" ht="43.2">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -667,53 +684,60 @@
         <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" t="s">
         <v>48</v>
-      </c>
-      <c r="C6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="28.8">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1696,14 +1720,13 @@
     <row r="991" ht="14.25" customHeight="1"/>
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{EB7444D4-9CFA-4278-A2ED-0B4E09293390}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1711,7 +1734,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2822,7 +2847,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2871,32 +2896,32 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -2904,10 +2929,10 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -2915,10 +2940,10 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
@@ -2926,10 +2951,10 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
update config and exception
</commit_message>
<xml_diff>
--- a/RPATemplete/Data/Config.xlsx
+++ b/RPATemplete/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thaibev\RPATemplete\RPATemplete\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA869FC-EFD7-41F4-B486-4F4105BDF36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE20D5F0-0CB4-4F85-B9BD-235724A05E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1164" windowWidth="17928" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t xml:space="preserve">Dear All &lt;br/&gt;This is auto email from Master Templete Bot.&lt;br/&gt;Detail is : </t>
+  </si>
+  <si>
+    <t>MailException</t>
+  </si>
+  <si>
+    <t>parnupon.k@thaibev.com</t>
   </si>
 </sst>
 </file>
@@ -254,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -264,6 +270,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,7 +588,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B15"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1711,7 +1718,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1835,7 +1844,14 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>